<commit_message>
earnings and employment data update
</commit_message>
<xml_diff>
--- a/data/historical/source/unemployment_historical.xlsx
+++ b/data/historical/source/unemployment_historical.xlsx
@@ -178,7 +178,7 @@
     <t>Wyoming</t>
   </si>
   <si>
-    <t>Unemployment Rate: January 1976 -- April 2016</t>
+    <t>Unemployment Rate: January 1976 -- May 2016</t>
   </si>
 </sst>
 </file>
@@ -1637,7 +1637,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A474" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J481" sqref="J481"/>
+      <selection pane="bottomLeft" activeCell="F493" sqref="F493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -79693,7 +79693,7 @@
         <v>3.8</v>
       </c>
       <c r="T489" s="2">
-        <v>5.3</v>
+        <v>5.4</v>
       </c>
       <c r="U489" s="2">
         <v>6.3</v>
@@ -79759,7 +79759,7 @@
         <v>5.3</v>
       </c>
       <c r="AP489" s="2">
-        <v>5.3</v>
+        <v>5.4</v>
       </c>
       <c r="AQ489" s="2">
         <v>5.8</v>
@@ -79796,7 +79796,165 @@
       </c>
     </row>
     <row r="490" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A490" s="6"/>
+      <c r="A490" s="6">
+        <v>42491</v>
+      </c>
+      <c r="B490" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="C490" s="2">
+        <v>6.1</v>
+      </c>
+      <c r="D490" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="E490" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="F490" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="G490" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="H490" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="I490" s="2">
+        <v>5.7</v>
+      </c>
+      <c r="J490" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K490" s="2">
+        <v>6.1</v>
+      </c>
+      <c r="L490" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="M490" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="N490" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="O490" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="P490" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="Q490" s="2">
+        <v>5</v>
+      </c>
+      <c r="R490" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="S490" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="T490" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="U490" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="V490" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="W490" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="X490" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="Y490" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="Z490" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="AA490" s="2">
+        <v>5.8</v>
+      </c>
+      <c r="AB490" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="AC490" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="AD490" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE490" s="2">
+        <v>6.1</v>
+      </c>
+      <c r="AF490" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="AG490" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AH490" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="AI490" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="AJ490" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AK490" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="AL490" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AM490" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="AN490" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="AO490" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="AP490" s="2">
+        <v>5.4</v>
+      </c>
+      <c r="AQ490" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="AR490" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="AS490" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AT490" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AU490" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="AV490" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="AW490" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="AX490" s="2">
+        <v>5.8</v>
+      </c>
+      <c r="AY490" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="AZ490" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="BA490" s="2">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="491" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A491" s="6"/>

</xml_diff>